<commit_message>
.env wurde eingerichtet & .gitignore erstellt
</commit_message>
<xml_diff>
--- a/Data/Student Mandatory Modules Grades Data.xlsx
+++ b/Data/Student Mandatory Modules Grades Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamal\PycharmProjects\Master_Projekt\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Projekte\OptiModuls_MP_87\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87539E8-F870-4D72-BD2A-EDE68BA99EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA5CFDA-63CD-4D6C-AFC3-B7212AB56B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,24 +195,6 @@
     <t>Burn</t>
   </si>
   <si>
-    <t>Thery</t>
-  </si>
-  <si>
-    <t>Beckberg</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Maxmann</t>
-  </si>
-  <si>
     <t>Louisa</t>
   </si>
   <si>
@@ -223,6 +205,24 @@
   </si>
   <si>
     <t>Ackermann</t>
+  </si>
+  <si>
+    <t>Kamal</t>
+  </si>
+  <si>
+    <t>Badawi</t>
+  </si>
+  <si>
+    <t>Khadija</t>
+  </si>
+  <si>
+    <t>Lamcharek</t>
+  </si>
+  <si>
+    <t>Ibrahim</t>
+  </si>
+  <si>
+    <t>Al-Showiter</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,8 +256,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF737677"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00ACFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +293,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -350,12 +369,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -365,15 +384,21 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,9 +414,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -429,9 +454,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,26 +489,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,26 +524,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -709,47 +700,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="56.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -841,7 +832,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -912,7 +903,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -992,7 +983,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1066,7 +1057,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1149,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1342,7 +1333,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1419,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1496,7 +1487,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1576,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1653,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1745,7 +1736,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +1813,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>52</v>
       </c>
@@ -1914,12 +1905,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8">
         <v>36539</v>
@@ -2006,12 +1997,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C16" s="8">
         <v>36540</v>
@@ -2098,12 +2089,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C17" s="8">
         <v>36541</v>
@@ -2190,12 +2181,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C18" s="8">
         <v>36542</v>
@@ -2282,12 +2273,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C19" s="8">
         <v>36543</v>
@@ -2373,6 +2364,10 @@
       <c r="AD19">
         <v>53</v>
       </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>